<commit_message>
Interacciones lmm y mlg
</commit_message>
<xml_diff>
--- a/MODELOS/variables predictoras.xlsx
+++ b/MODELOS/variables predictoras.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="34">
   <si>
     <t>Variable</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>Frecuencia para hablar de problemas con familiares o amigos</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>s12_l</t>
+  </si>
+  <si>
+    <t>s04_l</t>
+  </si>
+  <si>
+    <t>s_imc_l</t>
   </si>
 </sst>
 </file>
@@ -432,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,7 +456,7 @@
     <col min="3" max="3" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,8 +478,11 @@
       <c r="G1">
         <v>2019</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -489,8 +504,11 @@
       <c r="G2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -512,8 +530,11 @@
       <c r="G3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -535,8 +556,11 @@
       <c r="G4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -558,8 +582,11 @@
       <c r="G5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -581,8 +608,11 @@
       <c r="G6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -604,8 +634,11 @@
       <c r="G7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -626,6 +659,9 @@
       </c>
       <c r="G8" t="s">
         <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>